<commit_message>
feature: image for tutorial
</commit_message>
<xml_diff>
--- a/script/dist/database/main_database_MU.xlsx
+++ b/script/dist/database/main_database_MU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahim Hadi Maula\Documents\No Party\07 - Freelance\GUI4Meeting\script\dist\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8634FC6-28C3-4042-A626-CF0D2CE08340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC36FC8C-6032-4645-AB43-86B81E6E7669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="192">
   <si>
     <t>event_code</t>
   </si>
@@ -1005,8 +1005,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1113,6 +1116,12 @@
       <c r="L2" t="s">
         <v>161</v>
       </c>
+      <c r="M2" t="s">
+        <v>161</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>161</v>
+      </c>
       <c r="P2" s="1">
         <v>43665.583333333343</v>
       </c>
@@ -1152,6 +1161,12 @@
         <v>161</v>
       </c>
       <c r="L3" t="s">
+        <v>161</v>
+      </c>
+      <c r="M3" t="s">
+        <v>161</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>161</v>
       </c>
       <c r="P3" s="1">

</xml_diff>